<commit_message>
Revised templates with links to datasets in GBIF.org
</commit_message>
<xml_diff>
--- a/gbif-ipt-docs/downloads/checklist_ipt_template_v1_example_data.xlsx
+++ b/gbif-ipt-docs/downloads/checklist_ipt_template_v1_example_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Classification" sheetId="2" r:id="rId1"/>
@@ -346,7 +346,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="174">
   <si>
     <t>taxonID</t>
   </si>
@@ -917,6 +917,12 @@
   </si>
   <si>
     <t>Equisetum variegatum subsp. alaskanum (A.A. Eaton) Hultén</t>
+  </si>
+  <si>
+    <t>http://www.gbif.org/dataset/3f8a1297-3259-4700-91fc-acc4170b27ce</t>
+  </si>
+  <si>
+    <t>The Database of Vascular Plants of Canada is used in building the GBIF Backbone Taxonomy. To see how GBIF indexes the data go here:</t>
   </si>
 </sst>
 </file>
@@ -1644,7 +1650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -3386,9 +3392,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -3438,74 +3444,91 @@
       <c r="A8" s="6"/>
       <c r="B8" s="9"/>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="30">
       <c r="A9" s="6"/>
-      <c r="B9" s="21" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="42">
+      <c r="B9" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="6"/>
-      <c r="B10" s="10" t="s">
-        <v>150</v>
+      <c r="B10" s="20" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="6"/>
-      <c r="B11" s="10"/>
-    </row>
-    <row r="12" spans="1:2" ht="16" thickBot="1">
-      <c r="A12" s="11" t="s">
+      <c r="B11" s="20"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="21" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="42">
+      <c r="A13" s="6"/>
+      <c r="B13" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="6"/>
+      <c r="B14" s="10"/>
+    </row>
+    <row r="15" spans="1:2" ht="16" thickBot="1">
+      <c r="A15" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B15" s="12" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="45">
-      <c r="A13" s="13" t="s">
+    <row r="16" spans="1:2" ht="45">
+      <c r="A16" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B16" s="14" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="15"/>
-      <c r="B14" s="14"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="15"/>
+      <c r="B17" s="14"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="16"/>
+      <c r="B18" s="17" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="30">
-      <c r="A16" s="3"/>
-      <c r="B16" s="18" t="s">
+    <row r="19" spans="1:2" ht="30">
+      <c r="A19" s="3"/>
+      <c r="B19" s="18" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="30">
-      <c r="A17" s="3"/>
-      <c r="B17" s="17" t="s">
+    <row r="20" spans="1:2" ht="30">
+      <c r="A20" s="3"/>
+      <c r="B20" s="17" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="17" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="17" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="B19" s="22" t="s">
+    <row r="22" spans="1:2">
+      <c r="B22" s="22" t="s">
         <v>152</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B10" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>